<commit_message>
it works. holy shit
</commit_message>
<xml_diff>
--- a/spec/arc-furnace/resources/other_excel.xlsx
+++ b/spec/arc-furnace/resources/other_excel.xlsx
@@ -381,7 +381,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -402,7 +402,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -413,7 +413,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -432,7 +432,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -453,7 +453,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -464,7 +464,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>

</xml_diff>